<commit_message>
Adding SQL practice examples
</commit_message>
<xml_diff>
--- a/src/com/skillstorm/week12/day2/sql-practice.xlsx
+++ b/src/com/skillstorm/week12/day2/sql-practice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Carter\Documents\workspace-spring-tool-suite-4-4.13.0.RELEASE\Training\src\com\skillstorm\week12\day2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C019C54D-5E42-43F8-97EE-5C3092C5FCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FB8B16-C768-4112-81C0-87F0850DE030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PK Practice" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="143">
   <si>
     <t>Student</t>
   </si>
@@ -450,6 +450,24 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Candidate Key</t>
+  </si>
+  <si>
+    <t>Primary Key</t>
+  </si>
+  <si>
+    <t>Natural Key</t>
+  </si>
+  <si>
+    <t>Aritificial Key</t>
   </si>
 </sst>
 </file>
@@ -558,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -569,6 +587,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -853,7 +872,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:O8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1453,7 +1472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC59DAD4-8228-46E8-942E-58CE80504B9C}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1843,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71292F5-D39A-4875-BE54-B4847CEDCB19}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1870,7 +1891,7 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1891,6 +1912,9 @@
       <c r="G2" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="J2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1914,6 +1938,9 @@
       <c r="G3">
         <v>63</v>
       </c>
+      <c r="J3" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -1936,6 +1963,9 @@
       </c>
       <c r="G4">
         <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1960,6 +1990,9 @@
       <c r="G5">
         <v>63</v>
       </c>
+      <c r="J5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -2037,7 +2070,7 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="9" t="s">
         <v>90</v>
       </c>
       <c r="L16" s="2" t="s">
@@ -2094,7 +2127,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2210,10 +2243,10 @@
       <c r="F23">
         <v>78</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="9" t="s">
         <v>90</v>
       </c>
       <c r="L23" s="2" t="s">
@@ -2342,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05613A99-B472-4FEB-90E8-2D23225C1E52}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2365,7 +2398,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2377,7 +2410,7 @@
       <c r="D2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>110</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -2672,6 +2705,17 @@
         <v>118</v>
       </c>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>124</v>
@@ -2705,6 +2749,9 @@
       <c r="J24" s="2" t="s">
         <v>125</v>
       </c>
+      <c r="K24" s="10" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -2728,6 +2775,9 @@
       <c r="J25" t="s">
         <v>126</v>
       </c>
+      <c r="K25">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -2751,6 +2801,9 @@
       <c r="J26" t="s">
         <v>127</v>
       </c>
+      <c r="K26">
+        <v>4.25</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -2774,6 +2827,9 @@
       <c r="J27" t="s">
         <v>128</v>
       </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -2796,6 +2852,9 @@
       </c>
       <c r="J28" t="s">
         <v>129</v>
+      </c>
+      <c r="K28">
+        <v>2.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -2828,5 +2887,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding SQL practice and SQL join examples
</commit_message>
<xml_diff>
--- a/src/com/skillstorm/week12/day2/sql-practice.xlsx
+++ b/src/com/skillstorm/week12/day2/sql-practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Carter\Documents\workspace-spring-tool-suite-4-4.13.0.RELEASE\Training\src\com\skillstorm\week12\day2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FB8B16-C768-4112-81C0-87F0850DE030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3DEAB4-8145-4857-9326-73FBAEDADB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="148">
   <si>
     <t>Student</t>
   </si>
@@ -468,6 +468,21 @@
   </si>
   <si>
     <t>Aritificial Key</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Salesperson</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Vegas</t>
+  </si>
+  <si>
+    <t>NV</t>
   </si>
 </sst>
 </file>
@@ -1864,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71292F5-D39A-4875-BE54-B4847CEDCB19}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2180,6 +2195,21 @@
       <c r="F20">
         <v>63</v>
       </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20" t="s">
+        <v>147</v>
+      </c>
+      <c r="M20" t="s">
+        <v>145</v>
+      </c>
+      <c r="N20" t="s">
+        <v>146</v>
+      </c>
+      <c r="O20">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -2312,6 +2342,24 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>78</v>
+      </c>
       <c r="J26" t="s">
         <v>78</v>
       </c>

</xml_diff>